<commit_message>
Add ImportExcel for Form 4.1
</commit_message>
<xml_diff>
--- a/data/Excel/4.1.xlsx
+++ b/data/Excel/4.1.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>№ п/п</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>За (год)</t>
+  </si>
+  <si>
+    <t>Код субъекта Российской Федерации</t>
+  </si>
+  <si>
+    <t>Номер корректировки</t>
   </si>
 </sst>
 </file>
@@ -262,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -384,11 +390,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -474,6 +489,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -793,10 +811,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:B35"/>
+  <dimension ref="A2:B35"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -805,22 +823,32 @@
     <col min="3" max="16384" width="11.25" style="9"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="23"/>
-    </row>
-    <row r="7" spans="1:2" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="6" spans="1:2" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B6" s="22"/>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="16"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -971,10 +999,10 @@
       <c r="B35" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rBnO/pT9deAfPKb1RcbbARlquwTVtZg1PRt3DpZJMjTfKh5kQeqLLzh5H/hxnWIpPR2oyxrqkyWkbDTbS9QkmA==" saltValue="FcsmmgZU6R599hOCXglBkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatRows="0" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection formatRows="0" insertRows="0" deleteRows="0" selectLockedCells="1"/>
   <mergeCells count="5">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A27:B27"/>
@@ -990,11 +1018,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:I26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1002,6 +1028,12 @@
     <col min="10" max="16384" width="11.25" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
     <row r="3" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="I3" s="19" t="s">
         <v>13</v>

</xml_diff>